<commit_message>
fix: rangoli app design
</commit_message>
<xml_diff>
--- a/sheets/ice-ta-rangoli.xlsx
+++ b/sheets/ice-ta-rangoli.xlsx
@@ -53,6 +53,138 @@
     <t>source</t>
   </si>
   <si>
+    <t>10 dots - bhogi kundalu designs -</t>
+  </si>
+  <si>
+    <t>https://img.youtube.com/vi/ter_4S1IT74/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ter_4S1IT74&amp;index=13&amp;list=PLKRWLFbODx6x7i2ShWMHPQ9DSoosA1-dz</t>
+  </si>
+  <si>
+    <t>ter_4S1IT74</t>
+  </si>
+  <si>
+    <t>S2 Kolam</t>
+  </si>
+  <si>
+    <t>pongal pot kolam with 15 dots.</t>
+  </si>
+  <si>
+    <t>https://img.youtube.com/vi/1C_XHct1RCI/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=1C_XHct1RCI&amp;list=PLKRWLFbODx6x7i2ShWMHPQ9DSoosA1-dz&amp;index=12</t>
+  </si>
+  <si>
+    <t>1C_XHct1RCI</t>
+  </si>
+  <si>
+    <t>bhogi kundalu muggulu</t>
+  </si>
+  <si>
+    <t>https://img.youtube.com/vi/sru-rG2ldK4/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=sru-rG2ldK4&amp;list=PLKRWLFbODx6x7i2ShWMHPQ9DSoosA1-dz&amp;index=11</t>
+  </si>
+  <si>
+    <t>sru-rG2ldK4</t>
+  </si>
+  <si>
+    <t>Pongal pot rangoli design with 12 dots.</t>
+  </si>
+  <si>
+    <t>https://img.youtube.com/vi/uOdaCSix7AI/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=uOdaCSix7AI&amp;list=PLKRWLFbODx6x7i2ShWMHPQ9DSoosA1-dz&amp;index=10</t>
+  </si>
+  <si>
+    <t>uOdaCSix7AI</t>
+  </si>
+  <si>
+    <t>easy bhogi kundalu designs</t>
+  </si>
+  <si>
+    <t>https://img.youtube.com/vi/Gzi_kZspV0M/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Gzi_kZspV0M&amp;list=PLKRWLFbODx6x7i2ShWMHPQ9DSoosA1-dz&amp;index=6</t>
+  </si>
+  <si>
+    <t>Gzi_kZspV0M</t>
+  </si>
+  <si>
+    <t>kundalu muggulu with 13 dots</t>
+  </si>
+  <si>
+    <t>https://img.youtube.com/vi/ZOB9vicTe-Y/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ZOB9vicTe-Y&amp;index=4&amp;list=PLKRWLFbODx6x7i2ShWMHPQ9DSoosA1-dz</t>
+  </si>
+  <si>
+    <t>ZOB9vicTe-Y</t>
+  </si>
+  <si>
+    <t>Pongal Bhogi Pot With Colours</t>
+  </si>
+  <si>
+    <t>https://img.youtube.com/vi/KyZpZj67QZU/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=KyZpZj67QZU&amp;list=PLlzpegbwatcN4wxBMPibctD-PPXfYd8BX</t>
+  </si>
+  <si>
+    <t>KyZpZj67QZU</t>
+  </si>
+  <si>
+    <t>Rangoli By Maya</t>
+  </si>
+  <si>
+    <t>pongal kolam sankranti rangoli</t>
+  </si>
+  <si>
+    <t>https://img.youtube.com/vi/2cKgclw3Rv8/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=2cKgclw3Rv8</t>
+  </si>
+  <si>
+    <t>2cKgclw3Rv8</t>
+  </si>
+  <si>
+    <t>muggulu rangoli</t>
+  </si>
+  <si>
+    <t>Bhogi Kundala Muggu With Dots</t>
+  </si>
+  <si>
+    <t>https://img.youtube.com/vi/ndnnPg4dxBQ/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ndnnPg4dxBQ</t>
+  </si>
+  <si>
+    <t>ndnnPg4dxBQ</t>
+  </si>
+  <si>
+    <t>Fashion World</t>
+  </si>
+  <si>
+    <t>Muggulu With 17 x 3 x 3 Straight Dots</t>
+  </si>
+  <si>
+    <t>https://img.youtube.com/vi/xfXpREzp0p8/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=xfXpREzp0p8</t>
+  </si>
+  <si>
+    <t>xfXpREzp0p8</t>
+  </si>
+  <si>
     <t>muggulu for new year</t>
   </si>
   <si>
@@ -182,138 +314,6 @@
     <t>DdjG57m-xh4</t>
   </si>
   <si>
-    <t>muggulu rangoli</t>
-  </si>
-  <si>
-    <t>10 dots - bhogi kundalu designs -</t>
-  </si>
-  <si>
-    <t>https://img.youtube.com/vi/ter_4S1IT74/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=ter_4S1IT74&amp;index=13&amp;list=PLKRWLFbODx6x7i2ShWMHPQ9DSoosA1-dz</t>
-  </si>
-  <si>
-    <t>ter_4S1IT74</t>
-  </si>
-  <si>
-    <t>S2 Kolam</t>
-  </si>
-  <si>
-    <t>pongal pot kolam with 15 dots.</t>
-  </si>
-  <si>
-    <t>https://img.youtube.com/vi/1C_XHct1RCI/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=1C_XHct1RCI&amp;list=PLKRWLFbODx6x7i2ShWMHPQ9DSoosA1-dz&amp;index=12</t>
-  </si>
-  <si>
-    <t>1C_XHct1RCI</t>
-  </si>
-  <si>
-    <t>bhogi kundalu muggulu</t>
-  </si>
-  <si>
-    <t>https://img.youtube.com/vi/sru-rG2ldK4/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=sru-rG2ldK4&amp;list=PLKRWLFbODx6x7i2ShWMHPQ9DSoosA1-dz&amp;index=11</t>
-  </si>
-  <si>
-    <t>sru-rG2ldK4</t>
-  </si>
-  <si>
-    <t>Pongal pot rangoli design with 12 dots.</t>
-  </si>
-  <si>
-    <t>https://img.youtube.com/vi/uOdaCSix7AI/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=uOdaCSix7AI&amp;list=PLKRWLFbODx6x7i2ShWMHPQ9DSoosA1-dz&amp;index=10</t>
-  </si>
-  <si>
-    <t>uOdaCSix7AI</t>
-  </si>
-  <si>
-    <t>easy bhogi kundalu designs</t>
-  </si>
-  <si>
-    <t>https://img.youtube.com/vi/Gzi_kZspV0M/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=Gzi_kZspV0M&amp;list=PLKRWLFbODx6x7i2ShWMHPQ9DSoosA1-dz&amp;index=6</t>
-  </si>
-  <si>
-    <t>Gzi_kZspV0M</t>
-  </si>
-  <si>
-    <t>kundalu muggulu with 13 dots</t>
-  </si>
-  <si>
-    <t>https://img.youtube.com/vi/ZOB9vicTe-Y/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=ZOB9vicTe-Y&amp;index=4&amp;list=PLKRWLFbODx6x7i2ShWMHPQ9DSoosA1-dz</t>
-  </si>
-  <si>
-    <t>ZOB9vicTe-Y</t>
-  </si>
-  <si>
-    <t>Pongal Bhogi Pot With Colours</t>
-  </si>
-  <si>
-    <t>https://img.youtube.com/vi/KyZpZj67QZU/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=KyZpZj67QZU&amp;list=PLlzpegbwatcN4wxBMPibctD-PPXfYd8BX</t>
-  </si>
-  <si>
-    <t>KyZpZj67QZU</t>
-  </si>
-  <si>
-    <t>Rangoli By Maya</t>
-  </si>
-  <si>
-    <t>pongal kolam sankranti rangoli</t>
-  </si>
-  <si>
-    <t>https://img.youtube.com/vi/2cKgclw3Rv8/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=2cKgclw3Rv8</t>
-  </si>
-  <si>
-    <t>2cKgclw3Rv8</t>
-  </si>
-  <si>
-    <t>Bhogi Kundala Muggu With Dots</t>
-  </si>
-  <si>
-    <t>https://img.youtube.com/vi/ndnnPg4dxBQ/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=ndnnPg4dxBQ</t>
-  </si>
-  <si>
-    <t>ndnnPg4dxBQ</t>
-  </si>
-  <si>
-    <t>Fashion World</t>
-  </si>
-  <si>
-    <t>Muggulu With 17 x 3 x 3 Straight Dots</t>
-  </si>
-  <si>
-    <t>https://img.youtube.com/vi/xfXpREzp0p8/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=xfXpREzp0p8</t>
-  </si>
-  <si>
-    <t>xfXpREzp0p8</t>
-  </si>
-  <si>
     <t>pulli kolam | 9 dots sikku kolam</t>
   </si>
   <si>
@@ -818,1048 +818,1135 @@
     <t>easy rangoli designs</t>
   </si>
   <si>
+    <t>6wmY90tkzuI</t>
+  </si>
+  <si>
+    <t>Latest simple flower rangoli designs | 7 to 4 dots</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/D7UO9z9KDFg/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/D7UO9z9KDFg</t>
+  </si>
+  <si>
+    <t>D7UO9z9KDFg</t>
+  </si>
+  <si>
+    <t>simple rangol</t>
+  </si>
+  <si>
+    <t>Rose flower kolam designs with 7x4 dots</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/PKUNQSJjGkw/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/PKUNQSJjGkw</t>
+  </si>
+  <si>
+    <t>PKUNQSJjGkw</t>
+  </si>
+  <si>
+    <t>Latest freehand kolam</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/EaB8SsrZZ0s/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/EaB8SsrZZ0s</t>
+  </si>
+  <si>
+    <t>EaB8SsrZZ0s</t>
+  </si>
+  <si>
+    <t>Beautiful and unique rangoli design</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/y44KK2ugc60/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/y44KK2ugc60</t>
+  </si>
+  <si>
+    <t>y44KK2ugc60</t>
+  </si>
+  <si>
+    <t>Poonam Borkar</t>
+  </si>
+  <si>
+    <t>Freehand Rangoli Designs with colours</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/2ccsotwQABA/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/2ccsotwQABA</t>
+  </si>
+  <si>
+    <t>2ccsotwQABA</t>
+  </si>
+  <si>
+    <t>Shital Daga</t>
+  </si>
+  <si>
+    <t>Simple freehand Rangoli design</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/vYmC3Y9I-hg/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/vYmC3Y9I-hg</t>
+  </si>
+  <si>
+    <t>vYmC3Y9I-hg</t>
+  </si>
+  <si>
+    <t>Easy freehand Muggulu design</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/0ygWtAJRTuA/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/0ygWtAJRTuA</t>
+  </si>
+  <si>
+    <t>0ygWtAJRTuA</t>
+  </si>
+  <si>
+    <t>Quick freehand Kolam</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/z4R9Uw7dVfg/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/z4R9Uw7dVfg</t>
+  </si>
+  <si>
+    <t>z4R9Uw7dVfg</t>
+  </si>
+  <si>
+    <t>Freehand rangoli designs with colours</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/BY3roEOUKNA/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/NhXUCsJm604/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/BY3roEOUKNA</t>
+  </si>
+  <si>
+    <t>BY3roEOUKNA</t>
+  </si>
+  <si>
+    <t>https://youtu.be/NhXUCsJm604</t>
+  </si>
+  <si>
+    <t>NhXUCsJm604</t>
+  </si>
+  <si>
+    <t>Rangoli design, colourful and beautiful</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/IBnFvSY1i8U/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/IBnFvSY1i8U</t>
+  </si>
+  <si>
+    <t>IBnFvSY1i8U</t>
+  </si>
+  <si>
+    <t>DEEPIKA RANGOLI AND ART</t>
+  </si>
+  <si>
+    <t>Beautiful Rainbow Rangoli Designs With Colours</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/iDWs8nGcXEk/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/iDWs8nGcXEk</t>
+  </si>
+  <si>
+    <t>iDWs8nGcXEk</t>
+  </si>
+  <si>
+    <t>2 easy small multicolored rangoli designs</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/hiLfJsx9zQU/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/hiLfJsx9zQU</t>
+  </si>
+  <si>
+    <t>hiLfJsx9zQU</t>
+  </si>
+  <si>
+    <t>easy rangoli for beginners</t>
+  </si>
+  <si>
+    <t>Innovative Daily Rangoli Designs</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/NkRZlY9OTLg/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/NkRZlY9OTLg</t>
+  </si>
+  <si>
+    <t>NkRZlY9OTLg</t>
+  </si>
+  <si>
+    <t>Shital Mahajan</t>
+  </si>
+  <si>
+    <t>Innovative Rangoli Designs Using CD and Bangles</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/7IVYpHMBfbE/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/7IVYpHMBfbE</t>
+  </si>
+  <si>
+    <t>7IVYpHMBfbE</t>
+  </si>
+  <si>
+    <t>Birds kolam designs with 5x3 dots</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/ZksVIwbFU8A/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/ZksVIwbFU8A</t>
+  </si>
+  <si>
+    <t>ZksVIwbFU8A&amp;t</t>
+  </si>
+  <si>
+    <t>beautiful peacock kolam designs with 7x4 dots</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/yAeBRQErUOQ/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/yAeBRQErUOQ</t>
+  </si>
+  <si>
+    <t>yAeBRQErUOQ</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/kbazjyy7nW4/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/kbazjyy7nW4</t>
+  </si>
+  <si>
+    <t>kbazjyy7nW4</t>
+  </si>
+  <si>
+    <t>kolam with 7 dots and 6 birds</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/ULRQVTxKNVI/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/ULRQVTxKNVI</t>
+  </si>
+  <si>
+    <t>ULRQVTxKNVI</t>
+  </si>
+  <si>
+    <t>Bird Rangoli Kolam Designs with 6x4 Dots</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/pu6ZynK1Uiw/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/pu6ZynK1Uiw</t>
+  </si>
+  <si>
+    <t>pu6ZynK1Uiw</t>
+  </si>
+  <si>
+    <t>4 to 4 dots birds kolam designs</t>
+  </si>
+  <si>
+    <t>https://youtu.be/EpqHe9lApVY</t>
+  </si>
+  <si>
+    <t>EpqHe9lApVY</t>
+  </si>
+  <si>
+    <t>modern kolam with dots</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/Kcjwl39D6Ks/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/Kcjwl39D6Ks</t>
+  </si>
+  <si>
+    <t>Kcjwl39D6Ks</t>
+  </si>
+  <si>
+    <t>Flower Rangoli # Peacock Rangoli</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/Y9elOLXRHn8/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/Y9elOLXRHn8</t>
+  </si>
+  <si>
+    <t>Y9elOLXRHn8</t>
+  </si>
+  <si>
+    <t>Rangoli Arts &amp; Salad Decorations</t>
+  </si>
+  <si>
+    <t>Onam Pookalam</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/OXm5BcxnjnI/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/OXm5BcxnjnI</t>
+  </si>
+  <si>
+    <t>OXm5BcxnjnI</t>
+  </si>
+  <si>
+    <t>Friday Magazine</t>
+  </si>
+  <si>
+    <t>simple onam atha pookalam</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/AmNPprbICPQ/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/AmNPprbICPQ</t>
+  </si>
+  <si>
+    <t>AmNPprbICPQ</t>
+  </si>
+  <si>
+    <t>ABD AnyBody Can Draw</t>
+  </si>
+  <si>
+    <t>How to make a Onam pookalam</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/9zKF8Dnf9sw/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/9zKF8Dnf9sw</t>
+  </si>
+  <si>
+    <t>9zKF8Dnf9sw</t>
+  </si>
+  <si>
+    <t>tim thankachan</t>
+  </si>
+  <si>
+    <t>Making Onappookkalam</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/wsozvVUwa70/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/wsozvVUwa70</t>
+  </si>
+  <si>
+    <t>wsozvVUwa70</t>
+  </si>
+  <si>
+    <t>Deepa George</t>
+  </si>
+  <si>
+    <t>Make Flower Rangoli</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/tp3wwLvQOTE/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/tp3wwLvQOTE</t>
+  </si>
+  <si>
+    <t>tp3wwLvQOTE</t>
+  </si>
+  <si>
+    <t>Cinecurry Lifestyle</t>
+  </si>
+  <si>
+    <t>flower rangoli designs</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/QMs-RW7DbmA/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/QMs-RW7DbmA</t>
+  </si>
+  <si>
+    <t>QMs-RW7DbmA</t>
+  </si>
+  <si>
+    <t>Rangoli designs with colours // Arts and Crafts</t>
+  </si>
+  <si>
+    <t>Beautiful flower kolam with colors</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/IGTojrViJho/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/IGTojrViJho</t>
+  </si>
+  <si>
+    <t>IGTojrViJho</t>
+  </si>
+  <si>
+    <t>7x4 dots flower kolam designs with colors</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/cze3to9EfV4/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/cze3to9EfV4</t>
+  </si>
+  <si>
+    <t>cze3to9EfV4</t>
+  </si>
+  <si>
+    <t>Beautiful rangoli design with 7X4 middle dots</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/pXs5EidCUhM/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/pXs5EidCUhM</t>
+  </si>
+  <si>
+    <t>pXs5EidCUhM</t>
+  </si>
+  <si>
+    <t>rose flower kolam with 13x7 dots</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/LHf8IoR7Kuo/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/LHf8IoR7Kuo</t>
+  </si>
+  <si>
+    <t>LHf8IoR7Kuo</t>
+  </si>
+  <si>
+    <t>Sankranthi Flowers Kolam Designs With 13-7 middle</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/71YTUzGFvd4/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/71YTUzGFvd4</t>
+  </si>
+  <si>
+    <t>71YTUzGFvd4</t>
+  </si>
+  <si>
+    <t>flower kolam designs with 5 dots</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/17rX5E2VAck/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/17rX5E2VAck</t>
+  </si>
+  <si>
+    <t>17rX5E2VAck</t>
+  </si>
+  <si>
+    <t>simple rangoli festival arts with dots</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/4f3KCa_cDjc/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/4f3KCa_cDjc</t>
+  </si>
+  <si>
+    <t>4f3KCa_cDjc</t>
+  </si>
+  <si>
+    <t>Small Fish Kolam Designs With 11-1 Dots</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/voUw4jbAdvs/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/voUw4jbAdvs</t>
+  </si>
+  <si>
+    <t>voUw4jbAdvs</t>
+  </si>
+  <si>
+    <t>simple fish rangoli kolam.11*6 dots</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/_JQSmK6YNbw/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/_JQSmK6YNbw</t>
+  </si>
+  <si>
+    <t>JQSmK6YNbw</t>
+  </si>
+  <si>
+    <t>color rangoli</t>
+  </si>
+  <si>
+    <t>Sankranthi Simple Fish Kolam Designs With 15-8 middle</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/A6WMPqskr58/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/A6WMPqskr58</t>
+  </si>
+  <si>
+    <t>A6WMPqskr58</t>
+  </si>
+  <si>
+    <t>Dot kolam 9 to 9 straight with fish</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/akUWq8FYNPU/mqdefault.jpg?</t>
+  </si>
+  <si>
+    <t>https://youtu.be/akUWq8FYNPU</t>
+  </si>
+  <si>
+    <t>akUWq8FYNPU</t>
+  </si>
+  <si>
+    <t>Learn Kolam</t>
+  </si>
+  <si>
+    <t>easy kolam fish with dots 9 to 5</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/Cie_WpzXwS4/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/Cie_WpzXwS4</t>
+  </si>
+  <si>
+    <t>Cie_WpzXwS4</t>
+  </si>
+  <si>
+    <t>fish kolam designs with 5x3 dots</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/TCp4EWQKxCE/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/TCp4EWQKxCE</t>
+  </si>
+  <si>
+    <t>TCp4EWQKxCE</t>
+  </si>
+  <si>
+    <t>Easy Color Rangoli Design For HOLI Festival</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/1gPPU1vj304/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/1gPPU1vj304</t>
+  </si>
+  <si>
+    <t>1gPPU1vj304</t>
+  </si>
+  <si>
+    <t>Pakka Local</t>
+  </si>
+  <si>
+    <t>Colorful Holi Special Rangoli</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/aMIOjhjnUok/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/aMIOjhjnUok</t>
+  </si>
+  <si>
+    <t>aMIOjhjnUok</t>
+  </si>
+  <si>
+    <t>Rangoli &amp; Art</t>
+  </si>
+  <si>
+    <t>simple kolam designs with 7x3 dots</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/G64iGZ7PIU4/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/G64iGZ7PIU4</t>
+  </si>
+  <si>
+    <t>G64iGZ7PIU4</t>
+  </si>
+  <si>
+    <t>Rangoli Design with colours for fesitvals and competitions with dots</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/OKDdWOgz6mo/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/OKDdWOgz6mo</t>
+  </si>
+  <si>
+    <t>OKDdWOgz6mo</t>
+  </si>
+  <si>
+    <t>Rangoli design with Colours Competitions With dots 11x6</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/3P3vt6M2His/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/3P3vt6M2His</t>
+  </si>
+  <si>
+    <t>3P3vt6M2His</t>
+  </si>
+  <si>
+    <t>Easy Colourful Rangoli Design for Festivals with dots 13x7</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/RFA8wIdDQcc/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/RFA8wIdDQcc</t>
+  </si>
+  <si>
+    <t>RFA8wIdDQcc</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>details</t>
+  </si>
+  <si>
+    <t>Pulli Kolam | Dotted Kolam</t>
+  </si>
+  <si>
+    <t>pulli</t>
+  </si>
+  <si>
+    <t>Kolam, Muggulu, Rangoli, With colors, With dots</t>
+  </si>
+  <si>
+    <t>New Year Kolam</t>
+  </si>
+  <si>
+    <t>newyear</t>
+  </si>
+  <si>
+    <t>Pongal Kolam | Sankranthi Muggulu</t>
+  </si>
+  <si>
+    <t>pongal</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>Diwali Rangoli | Deepavali Kolam</t>
+  </si>
+  <si>
+    <t>diwali</t>
+  </si>
+  <si>
+    <t>Margazhi Kolam</t>
+  </si>
+  <si>
+    <t>margazhi</t>
+  </si>
+  <si>
+    <t>Flower Design Kolam</t>
+  </si>
+  <si>
+    <t>flower</t>
+  </si>
+  <si>
+    <t>Freehand Rangoli | Kolam without dots</t>
+  </si>
+  <si>
+    <t>freehand</t>
+  </si>
+  <si>
+    <t>Freehand Color Rangoli</t>
+  </si>
+  <si>
+    <t>freecolor</t>
+  </si>
+  <si>
+    <t>Birds Kolam</t>
+  </si>
+  <si>
+    <t>birds</t>
+  </si>
+  <si>
+    <t>Kolam with Flowers</t>
+  </si>
+  <si>
+    <t>withflowers</t>
+  </si>
+  <si>
+    <t>Onam Rangoli</t>
+  </si>
+  <si>
+    <t>onam</t>
+  </si>
+  <si>
+    <t>Fish Kolam</t>
+  </si>
+  <si>
+    <t>fish</t>
+  </si>
+  <si>
+    <t>Holi Rangoli</t>
+  </si>
+  <si>
+    <t>holi</t>
+  </si>
+  <si>
+    <t>Christmas Rangoli</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/kaJ97Hzz9J8/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>christmas</t>
+  </si>
+  <si>
+    <t>Sangu Kolam</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/U-G6rBKIM_k/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>sangu</t>
+  </si>
+  <si>
+    <t>Maha Shivaratri Kolam</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/C5pKc_8eGpQ/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>shiva</t>
+  </si>
+  <si>
+    <t>Vinayagar Chaturthi Kolam</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/fuqzN6iCKoI/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>vinayagar</t>
+  </si>
+  <si>
+    <t>Butterfly Rangoli</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/9JQVTQdqXS0/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>butterfly</t>
+  </si>
+  <si>
+    <t>karthigai Deepam Kolam</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/sPqNRUmLHi0/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>karthigai</t>
+  </si>
+  <si>
+    <t>Rose Kolam</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/ZtyXKiTDOtc/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>rose</t>
+  </si>
+  <si>
+    <t>Lotus Kolam</t>
+  </si>
+  <si>
+    <t>lotus</t>
+  </si>
+  <si>
+    <t>Peacock Kolam</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/A1dWDe6vLzo/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>peacock</t>
+  </si>
+  <si>
+    <t>Other Festival Kolam</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/XmnZ2Kj6dvU/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>others</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rama Navami, Saraswathi Pooja, Chitra Pournami, Aadi Perukku, Tamil new Year </t>
+  </si>
+  <si>
+    <t>Santa claus Rangoli with 21x14 straight Dots</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/Ooic3qT4PRA/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/Ooic3qT4PRA</t>
+  </si>
+  <si>
+    <t>Ooic3qT4PRA</t>
+  </si>
+  <si>
+    <t>Simple Christmas Rangoli Design with 5 Dots</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/3l2Ltp-28HI/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/3l2Ltp-28HI</t>
+  </si>
+  <si>
+    <t>3l2Ltp-28HI</t>
+  </si>
+  <si>
+    <t>Daily Rangoli Designs</t>
+  </si>
+  <si>
+    <t>Christmas Rangoli Design with colours &amp; dots 10x8</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/xe5Wsr78wq4/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/xe5Wsr78wq4</t>
+  </si>
+  <si>
+    <t>xe5Wsr78wq4</t>
+  </si>
+  <si>
+    <t>Christmas rangoli design</t>
+  </si>
+  <si>
+    <t>https://youtu.be/kaJ97Hzz9J8</t>
+  </si>
+  <si>
+    <t>kaJ97Hzz9J8</t>
+  </si>
+  <si>
+    <t>Christmas Special Kolam | 13×7 interlaced dots</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/k_0ZGa4vcpc/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/k_0ZGa4vcpc</t>
+  </si>
+  <si>
+    <t>k_0ZGa4vcpc</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/UHRy0sqUM1I/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/UHRy0sqUM1I</t>
+  </si>
+  <si>
+    <t>UHRy0sqUM1I</t>
+  </si>
+  <si>
+    <t>Christmas Rangoli Designs with 13x 7 Dots</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/i6jrBhddpaE/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/i6jrBhddpaE</t>
+  </si>
+  <si>
+    <t>i6jrBhddpaE</t>
+  </si>
+  <si>
+    <t>sangu kolam | 15*8 dots</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/COi3WRP0TNs/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/COi3WRP0TNs</t>
+  </si>
+  <si>
+    <t>COi3WRP0TNs</t>
+  </si>
+  <si>
+    <t>Sangu kolam</t>
+  </si>
+  <si>
+    <t>https://youtu.be/U-G6rBKIM_k</t>
+  </si>
+  <si>
+    <t>U-G6rBKIM_k</t>
+  </si>
+  <si>
+    <t>Rangoli New Design</t>
+  </si>
+  <si>
+    <t>Sangu kolam with dots/poo kolam with 7 to 1 dot</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/ZcmwXlw2MOk/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/ZcmwXlw2MOk</t>
+  </si>
+  <si>
+    <t>ZcmwXlw2MOk</t>
+  </si>
+  <si>
+    <t>5X1 middle dots</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/L5LEiGaeu1I/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/L5LEiGaeu1I</t>
+  </si>
+  <si>
+    <t>L5LEiGaeu1I</t>
+  </si>
+  <si>
+    <t>Latest 9-5 Inerlaced Dots Rangoli</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/b5bu_o-zy3k/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/b5bu_o-zy3k</t>
+  </si>
+  <si>
+    <t>b5bu_o-zy3k</t>
+  </si>
+  <si>
+    <t>Daily Rangoli</t>
+  </si>
+  <si>
+    <t>Festivals with dots 13x7</t>
+  </si>
+  <si>
+    <t>13x7 Easy Rainbow Rangoli</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/1Xmc9xb8A0s/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/1Xmc9xb8A0s</t>
+  </si>
+  <si>
+    <t>1Xmc9xb8A0s</t>
+  </si>
+  <si>
+    <t>17to17 dots rangoli for mahashivratri</t>
+  </si>
+  <si>
+    <t>https://youtu.be/C5pKc_8eGpQ</t>
+  </si>
+  <si>
+    <t>C5pKc_8eGpQ</t>
+  </si>
+  <si>
+    <t>Hemlata's Rangoli Designs</t>
+  </si>
+  <si>
+    <t>Special Shiva ratri Muggulu</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/GSRd1_aRxHo/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/GSRd1_aRxHo</t>
+  </si>
+  <si>
+    <t>GSRd1_aRxHo</t>
+  </si>
+  <si>
+    <t>Lovely Kolam</t>
+  </si>
+  <si>
+    <t>dots rangoli designs</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/68829aQjCs0/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/68829aQjCs0</t>
+  </si>
+  <si>
+    <t>68829aQjCs0</t>
+  </si>
+  <si>
+    <t>Easy 11x11 dots Shiva Lingam</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/Cw1w-p2foSU/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/Cw1w-p2foSU</t>
+  </si>
+  <si>
+    <t>Cw1w-p2foSU</t>
+  </si>
+  <si>
+    <t>Pedda Balashiksha</t>
+  </si>
+  <si>
+    <t>Shiva muggulu | kolam</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/-e2PxHvAUd0/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/-e2PxHvAUd0</t>
+  </si>
+  <si>
+    <t>e2PxHvAUd0</t>
+  </si>
+  <si>
+    <t>KRISHNASOUL</t>
+  </si>
+  <si>
+    <t>Kolam - 10x10 Dots</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/0CAQ5lWIg6M/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/0CAQ5lWIg6M</t>
+  </si>
+  <si>
+    <t>0CAQ5lWIg6M</t>
+  </si>
+  <si>
+    <t>Madhavi Creations TV</t>
+  </si>
+  <si>
     <t>6wmY90tkzuI&amp;t</t>
   </si>
   <si>
-    <t>Latest simple flower rangoli designs | 7 to 4 dots</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/D7UO9z9KDFg/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/D7UO9z9KDFg</t>
-  </si>
-  <si>
-    <t>D7UO9z9KDFg</t>
-  </si>
-  <si>
-    <t>simple rangol</t>
-  </si>
-  <si>
-    <t>Rose flower kolam designs with 7x4 dots</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/PKUNQSJjGkw/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/PKUNQSJjGkw</t>
-  </si>
-  <si>
-    <t>PKUNQSJjGkw</t>
-  </si>
-  <si>
-    <t>Latest freehand kolam</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/EaB8SsrZZ0s/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/EaB8SsrZZ0s</t>
-  </si>
-  <si>
-    <t>EaB8SsrZZ0s</t>
-  </si>
-  <si>
-    <t>Beautiful and unique rangoli design</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/y44KK2ugc60/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/y44KK2ugc60</t>
-  </si>
-  <si>
-    <t>y44KK2ugc60</t>
-  </si>
-  <si>
-    <t>Poonam Borkar</t>
-  </si>
-  <si>
-    <t>Freehand Rangoli Designs with colours</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/2ccsotwQABA/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/2ccsotwQABA</t>
-  </si>
-  <si>
-    <t>2ccsotwQABA</t>
-  </si>
-  <si>
-    <t>Shital Daga</t>
-  </si>
-  <si>
-    <t>Simple freehand Rangoli design</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/vYmC3Y9I-hg/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/vYmC3Y9I-hg</t>
-  </si>
-  <si>
-    <t>vYmC3Y9I-hg</t>
-  </si>
-  <si>
-    <t>Easy freehand Muggulu design</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/0ygWtAJRTuA/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/0ygWtAJRTuA</t>
-  </si>
-  <si>
-    <t>0ygWtAJRTuA</t>
-  </si>
-  <si>
-    <t>Quick freehand Kolam</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/z4R9Uw7dVfg/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/z4R9Uw7dVfg</t>
-  </si>
-  <si>
-    <t>z4R9Uw7dVfg</t>
-  </si>
-  <si>
-    <t>Freehand rangoli designs with colours</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/BY3roEOUKNA/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/BY3roEOUKNA</t>
-  </si>
-  <si>
-    <t>BY3roEOUKNA</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/NhXUCsJm604/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/NhXUCsJm604</t>
-  </si>
-  <si>
-    <t>NhXUCsJm604</t>
-  </si>
-  <si>
-    <t>Rangoli design, colourful and beautiful</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/IBnFvSY1i8U/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/IBnFvSY1i8U</t>
-  </si>
-  <si>
-    <t>IBnFvSY1i8U</t>
-  </si>
-  <si>
-    <t>DEEPIKA RANGOLI AND ART</t>
-  </si>
-  <si>
-    <t>Beautiful Rainbow Rangoli Designs With Colours</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/iDWs8nGcXEk/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/iDWs8nGcXEk</t>
-  </si>
-  <si>
-    <t>iDWs8nGcXEk</t>
-  </si>
-  <si>
-    <t>2 easy small multicolored rangoli designs</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/hiLfJsx9zQU/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/hiLfJsx9zQU</t>
-  </si>
-  <si>
-    <t>hiLfJsx9zQU</t>
-  </si>
-  <si>
-    <t>easy rangoli for beginners</t>
-  </si>
-  <si>
-    <t>Innovative Daily Rangoli Designs</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/NkRZlY9OTLg/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/NkRZlY9OTLg</t>
-  </si>
-  <si>
-    <t>NkRZlY9OTLg</t>
-  </si>
-  <si>
-    <t>Shital Mahajan</t>
-  </si>
-  <si>
-    <t>Innovative Rangoli Designs Using CD and Bangles</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/7IVYpHMBfbE/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/7IVYpHMBfbE</t>
-  </si>
-  <si>
-    <t>7IVYpHMBfbE</t>
-  </si>
-  <si>
-    <t>Birds kolam designs with 5x3 dots</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/ZksVIwbFU8A/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/ZksVIwbFU8A</t>
-  </si>
-  <si>
-    <t>ZksVIwbFU8A&amp;t</t>
-  </si>
-  <si>
-    <t>beautiful peacock kolam designs with 7x4 dots</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/yAeBRQErUOQ/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/yAeBRQErUOQ</t>
-  </si>
-  <si>
-    <t>yAeBRQErUOQ</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/kbazjyy7nW4/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/kbazjyy7nW4</t>
-  </si>
-  <si>
-    <t>kbazjyy7nW4</t>
-  </si>
-  <si>
-    <t>kolam with 7 dots and 6 birds</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/ULRQVTxKNVI/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/ULRQVTxKNVI</t>
-  </si>
-  <si>
-    <t>ULRQVTxKNVI</t>
-  </si>
-  <si>
-    <t>Bird Rangoli Kolam Designs with 6x4 Dots</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/pu6ZynK1Uiw/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/pu6ZynK1Uiw</t>
-  </si>
-  <si>
-    <t>pu6ZynK1Uiw</t>
-  </si>
-  <si>
-    <t>4 to 4 dots birds kolam designs</t>
-  </si>
-  <si>
-    <t>https://youtu.be/EpqHe9lApVY</t>
-  </si>
-  <si>
-    <t>EpqHe9lApVY</t>
-  </si>
-  <si>
-    <t>modern kolam with dots</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/Kcjwl39D6Ks/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/Kcjwl39D6Ks</t>
-  </si>
-  <si>
-    <t>Kcjwl39D6Ks</t>
-  </si>
-  <si>
-    <t>Flower Rangoli # Peacock Rangoli</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/Y9elOLXRHn8/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/Y9elOLXRHn8</t>
-  </si>
-  <si>
-    <t>Y9elOLXRHn8</t>
-  </si>
-  <si>
-    <t>Rangoli Arts &amp; Salad Decorations</t>
-  </si>
-  <si>
-    <t>Onam Pookalam</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/OXm5BcxnjnI/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/OXm5BcxnjnI</t>
-  </si>
-  <si>
-    <t>OXm5BcxnjnI</t>
-  </si>
-  <si>
-    <t>Friday Magazine</t>
-  </si>
-  <si>
-    <t>simple onam atha pookalam</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/AmNPprbICPQ/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/AmNPprbICPQ</t>
-  </si>
-  <si>
-    <t>AmNPprbICPQ</t>
-  </si>
-  <si>
-    <t>ABD AnyBody Can Draw</t>
-  </si>
-  <si>
-    <t>How to make a Onam pookalam</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/9zKF8Dnf9sw/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/9zKF8Dnf9sw</t>
-  </si>
-  <si>
-    <t>9zKF8Dnf9sw</t>
-  </si>
-  <si>
-    <t>tim thankachan</t>
-  </si>
-  <si>
-    <t>Making Onappookkalam</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/wsozvVUwa70/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/wsozvVUwa70</t>
-  </si>
-  <si>
-    <t>wsozvVUwa70</t>
-  </si>
-  <si>
-    <t>Deepa George</t>
-  </si>
-  <si>
-    <t>Make Flower Rangoli</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/tp3wwLvQOTE/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/tp3wwLvQOTE</t>
-  </si>
-  <si>
-    <t>tp3wwLvQOTE</t>
-  </si>
-  <si>
-    <t>Cinecurry Lifestyle</t>
-  </si>
-  <si>
-    <t>flower rangoli designs</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/QMs-RW7DbmA/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/QMs-RW7DbmA</t>
-  </si>
-  <si>
-    <t>QMs-RW7DbmA</t>
-  </si>
-  <si>
-    <t>Rangoli designs with colours // Arts and Crafts</t>
-  </si>
-  <si>
-    <t>Beautiful flower kolam with colors</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/IGTojrViJho/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/IGTojrViJho</t>
-  </si>
-  <si>
-    <t>IGTojrViJho</t>
-  </si>
-  <si>
-    <t>7x4 dots flower kolam designs with colors</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/cze3to9EfV4/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/cze3to9EfV4</t>
-  </si>
-  <si>
-    <t>cze3to9EfV4</t>
-  </si>
-  <si>
-    <t>Beautiful rangoli design with 7X4 middle dots</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/pXs5EidCUhM/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/pXs5EidCUhM</t>
-  </si>
-  <si>
-    <t>pXs5EidCUhM</t>
-  </si>
-  <si>
-    <t>rose flower kolam with 13x7 dots</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/LHf8IoR7Kuo/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/LHf8IoR7Kuo</t>
-  </si>
-  <si>
-    <t>LHf8IoR7Kuo</t>
-  </si>
-  <si>
-    <t>Sankranthi Flowers Kolam Designs With 13-7 middle</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/71YTUzGFvd4/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/71YTUzGFvd4</t>
-  </si>
-  <si>
-    <t>71YTUzGFvd4</t>
-  </si>
-  <si>
-    <t>flower kolam designs with 5 dots</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/17rX5E2VAck/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/17rX5E2VAck</t>
-  </si>
-  <si>
-    <t>17rX5E2VAck</t>
-  </si>
-  <si>
-    <t>simple rangoli festival arts with dots</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/4f3KCa_cDjc/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/4f3KCa_cDjc</t>
-  </si>
-  <si>
-    <t>4f3KCa_cDjc</t>
-  </si>
-  <si>
-    <t>Small Fish Kolam Designs With 11-1 Dots</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/voUw4jbAdvs/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/voUw4jbAdvs</t>
-  </si>
-  <si>
-    <t>voUw4jbAdvs</t>
-  </si>
-  <si>
-    <t>simple fish rangoli kolam.11*6 dots</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/_JQSmK6YNbw/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/_JQSmK6YNbw</t>
-  </si>
-  <si>
-    <t>JQSmK6YNbw</t>
-  </si>
-  <si>
-    <t>color rangoli</t>
-  </si>
-  <si>
-    <t>Sankranthi Simple Fish Kolam Designs With 15-8 middle</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/A6WMPqskr58/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/A6WMPqskr58</t>
-  </si>
-  <si>
-    <t>A6WMPqskr58</t>
-  </si>
-  <si>
-    <t>Dot kolam 9 to 9 straight with fish</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/akUWq8FYNPU/mqdefault.jpg?</t>
-  </si>
-  <si>
-    <t>https://youtu.be/akUWq8FYNPU</t>
-  </si>
-  <si>
-    <t>akUWq8FYNPU</t>
-  </si>
-  <si>
-    <t>Learn Kolam</t>
-  </si>
-  <si>
-    <t>easy kolam fish with dots 9 to 5</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/Cie_WpzXwS4/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/Cie_WpzXwS4</t>
-  </si>
-  <si>
-    <t>Cie_WpzXwS4</t>
-  </si>
-  <si>
-    <t>fish kolam designs with 5x3 dots</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/TCp4EWQKxCE/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/TCp4EWQKxCE</t>
-  </si>
-  <si>
-    <t>TCp4EWQKxCE</t>
-  </si>
-  <si>
-    <t>Easy Color Rangoli Design For HOLI Festival</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/1gPPU1vj304/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/1gPPU1vj304</t>
-  </si>
-  <si>
-    <t>1gPPU1vj304</t>
-  </si>
-  <si>
-    <t>Pakka Local</t>
-  </si>
-  <si>
-    <t>Colorful Holi Special Rangoli</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/aMIOjhjnUok/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/aMIOjhjnUok</t>
-  </si>
-  <si>
-    <t>aMIOjhjnUok</t>
-  </si>
-  <si>
-    <t>Rangoli &amp; Art</t>
-  </si>
-  <si>
-    <t>simple kolam designs with 7x3 dots</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/G64iGZ7PIU4/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/G64iGZ7PIU4</t>
-  </si>
-  <si>
-    <t>G64iGZ7PIU4</t>
-  </si>
-  <si>
-    <t>Rangoli Design with colours for fesitvals and competitions with dots</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/OKDdWOgz6mo/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/OKDdWOgz6mo</t>
-  </si>
-  <si>
-    <t>OKDdWOgz6mo</t>
-  </si>
-  <si>
-    <t>Rangoli design with Colours Competitions With dots 11x6</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/3P3vt6M2His/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/3P3vt6M2His</t>
-  </si>
-  <si>
-    <t>3P3vt6M2His</t>
-  </si>
-  <si>
-    <t>Easy Colourful Rangoli Design for Festivals with dots 13x7</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/RFA8wIdDQcc/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/RFA8wIdDQcc</t>
-  </si>
-  <si>
-    <t>RFA8wIdDQcc</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>details</t>
-  </si>
-  <si>
-    <t>Pulli Kolam | Dotted Kolam</t>
-  </si>
-  <si>
-    <t>pulli</t>
-  </si>
-  <si>
-    <t>Kolam, Muggulu, Rangoli, With colors, With dots</t>
-  </si>
-  <si>
-    <t>New Year Kolam</t>
-  </si>
-  <si>
-    <t>newyear</t>
-  </si>
-  <si>
-    <t>Pongal Kolam | Sankranthi Muggulu</t>
-  </si>
-  <si>
-    <t>pongal</t>
-  </si>
-  <si>
-    <t>color</t>
-  </si>
-  <si>
-    <t>Diwali Rangoli | Deepavali Kolam</t>
-  </si>
-  <si>
-    <t>diwali</t>
-  </si>
-  <si>
-    <t>Margazhi Kolam</t>
-  </si>
-  <si>
-    <t>margazhi</t>
-  </si>
-  <si>
-    <t>Flower Design Kolam</t>
-  </si>
-  <si>
-    <t>flower</t>
-  </si>
-  <si>
-    <t>Freehand Rangoli | Kolam without dots</t>
-  </si>
-  <si>
-    <t>freehand</t>
-  </si>
-  <si>
-    <t>Freehand Color Rangoli</t>
-  </si>
-  <si>
-    <t>freecolor</t>
-  </si>
-  <si>
-    <t>Birds Kolam</t>
-  </si>
-  <si>
-    <t>birds</t>
-  </si>
-  <si>
-    <t>Kolam with Flowers</t>
-  </si>
-  <si>
-    <t>withflowers</t>
-  </si>
-  <si>
-    <t>Onam Rangoli</t>
-  </si>
-  <si>
-    <t>onam</t>
-  </si>
-  <si>
-    <t>Fish Kolam</t>
-  </si>
-  <si>
-    <t>fish</t>
-  </si>
-  <si>
-    <t>Holi Rangoli</t>
-  </si>
-  <si>
-    <t>holi</t>
-  </si>
-  <si>
-    <t>Christmas Rangoli</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/kaJ97Hzz9J8/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>christmas</t>
-  </si>
-  <si>
-    <t>Sangu Kolam</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/U-G6rBKIM_k/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>sangu</t>
-  </si>
-  <si>
-    <t>Maha Shivaratri Kolam</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/C5pKc_8eGpQ/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>shiva</t>
-  </si>
-  <si>
-    <t>Vinayagar Chaturthi Kolam</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/fuqzN6iCKoI/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>vinayagar</t>
-  </si>
-  <si>
-    <t>Butterfly Rangoli</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/9JQVTQdqXS0/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>butterfly</t>
-  </si>
-  <si>
-    <t>karthigai Deepam Kolam</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/sPqNRUmLHi0/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>karthigai</t>
-  </si>
-  <si>
-    <t>Rose Kolam</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/ZtyXKiTDOtc/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>rose</t>
-  </si>
-  <si>
-    <t>Lotus Kolam</t>
-  </si>
-  <si>
-    <t>lotus</t>
-  </si>
-  <si>
-    <t>Peacock Kolam</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/A1dWDe6vLzo/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>peacock</t>
-  </si>
-  <si>
-    <t>Other Festival Kolam</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/XmnZ2Kj6dvU/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>others</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rama Navami, Saraswathi Pooja, Chitra Pournami, Aadi Perukku, Tamil new Year </t>
-  </si>
-  <si>
-    <t>Santa claus Rangoli with 21x14 straight Dots</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/Ooic3qT4PRA/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/Ooic3qT4PRA</t>
-  </si>
-  <si>
-    <t>Ooic3qT4PRA</t>
-  </si>
-  <si>
-    <t>Simple Christmas Rangoli Design with 5 Dots</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/3l2Ltp-28HI/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/3l2Ltp-28HI</t>
-  </si>
-  <si>
-    <t>3l2Ltp-28HI</t>
-  </si>
-  <si>
-    <t>Daily Rangoli Designs</t>
-  </si>
-  <si>
-    <t>Christmas Rangoli Design with colours &amp; dots 10x8</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/xe5Wsr78wq4/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/xe5Wsr78wq4</t>
-  </si>
-  <si>
-    <t>xe5Wsr78wq4</t>
-  </si>
-  <si>
-    <t>Christmas rangoli design</t>
-  </si>
-  <si>
-    <t>https://youtu.be/kaJ97Hzz9J8</t>
-  </si>
-  <si>
-    <t>kaJ97Hzz9J8</t>
-  </si>
-  <si>
-    <t>Christmas Special Kolam | 13×7 interlaced dots</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/k_0ZGa4vcpc/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/k_0ZGa4vcpc</t>
-  </si>
-  <si>
-    <t>k_0ZGa4vcpc</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/UHRy0sqUM1I/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/UHRy0sqUM1I</t>
-  </si>
-  <si>
-    <t>UHRy0sqUM1I</t>
-  </si>
-  <si>
-    <t>Christmas Rangoli Designs with 13x 7 Dots</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/i6jrBhddpaE/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/i6jrBhddpaE</t>
-  </si>
-  <si>
-    <t>i6jrBhddpaE</t>
-  </si>
-  <si>
-    <t>sangu kolam | 15*8 dots</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/COi3WRP0TNs/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/COi3WRP0TNs</t>
-  </si>
-  <si>
-    <t>COi3WRP0TNs</t>
-  </si>
-  <si>
-    <t>Sangu kolam</t>
-  </si>
-  <si>
-    <t>https://youtu.be/U-G6rBKIM_k</t>
-  </si>
-  <si>
-    <t>U-G6rBKIM_k</t>
-  </si>
-  <si>
-    <t>Rangoli New Design</t>
-  </si>
-  <si>
-    <t>Sangu kolam with dots/poo kolam with 7 to 1 dot</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/ZcmwXlw2MOk/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/ZcmwXlw2MOk</t>
-  </si>
-  <si>
-    <t>ZcmwXlw2MOk</t>
-  </si>
-  <si>
-    <t>5X1 middle dots</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/L5LEiGaeu1I/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/L5LEiGaeu1I</t>
-  </si>
-  <si>
-    <t>L5LEiGaeu1I</t>
-  </si>
-  <si>
-    <t>Latest 9-5 Inerlaced Dots Rangoli</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/b5bu_o-zy3k/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/b5bu_o-zy3k</t>
-  </si>
-  <si>
-    <t>b5bu_o-zy3k</t>
-  </si>
-  <si>
-    <t>Daily Rangoli</t>
-  </si>
-  <si>
-    <t>Festivals with dots 13x7</t>
-  </si>
-  <si>
-    <t>13x7 Easy Rainbow Rangoli</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/1Xmc9xb8A0s/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/1Xmc9xb8A0s</t>
-  </si>
-  <si>
-    <t>1Xmc9xb8A0s</t>
-  </si>
-  <si>
-    <t>17to17 dots rangoli for mahashivratri</t>
-  </si>
-  <si>
-    <t>https://youtu.be/C5pKc_8eGpQ</t>
-  </si>
-  <si>
-    <t>C5pKc_8eGpQ</t>
-  </si>
-  <si>
-    <t>Hemlata's Rangoli Designs</t>
-  </si>
-  <si>
-    <t>Special Shiva ratri Muggulu</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/GSRd1_aRxHo/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/GSRd1_aRxHo</t>
-  </si>
-  <si>
-    <t>GSRd1_aRxHo</t>
-  </si>
-  <si>
-    <t>Lovely Kolam</t>
-  </si>
-  <si>
-    <t>dots rangoli designs</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/68829aQjCs0/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/68829aQjCs0</t>
-  </si>
-  <si>
-    <t>68829aQjCs0</t>
-  </si>
-  <si>
-    <t>Easy 11x11 dots Shiva Lingam</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/Cw1w-p2foSU/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/Cw1w-p2foSU</t>
-  </si>
-  <si>
-    <t>Cw1w-p2foSU</t>
-  </si>
-  <si>
-    <t>Pedda Balashiksha</t>
-  </si>
-  <si>
-    <t>Shiva muggulu | kolam</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/-e2PxHvAUd0/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/-e2PxHvAUd0</t>
-  </si>
-  <si>
-    <t>e2PxHvAUd0</t>
-  </si>
-  <si>
-    <t>KRISHNASOUL</t>
-  </si>
-  <si>
-    <t>Kolam - 10x10 Dots</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/0CAQ5lWIg6M/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/0CAQ5lWIg6M</t>
-  </si>
-  <si>
-    <t>0CAQ5lWIg6M</t>
-  </si>
-  <si>
-    <t>Madhavi Creations TV</t>
+    <t>Beautiful Butterfly rangoli kolam |13*7 dots</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/sFyte69z454/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/sFyte69z454</t>
+  </si>
+  <si>
+    <t>sFyte69z454</t>
+  </si>
+  <si>
+    <t>simple butterfly kolam |13*7 dots</t>
+  </si>
+  <si>
+    <t>https://youtu.be/9JQVTQdqXS0</t>
+  </si>
+  <si>
+    <t>9JQVTQdqXS0</t>
+  </si>
+  <si>
+    <t>Rangoli Art | 7 to 4 Interlaced Dots</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/yzJ8lfMxlck/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/yzJ8lfMxlck</t>
+  </si>
+  <si>
+    <t>yzJ8lfMxlck</t>
+  </si>
+  <si>
+    <t>Simple Butterfly Rangoli Design with Colours &amp; dots 9x5</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/HnFDl171M4M/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/HnFDl171M4M</t>
+  </si>
+  <si>
+    <t>HnFDl171M4M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">simple flower rangoli with dots 12-2-2 </t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/KiCPCRXBOwo/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/KiCPCRXBOwo</t>
+  </si>
+  <si>
+    <t>KiCPCRXBOwo</t>
+  </si>
+  <si>
+    <t>Dheepiika Rangolis</t>
+  </si>
+  <si>
+    <t>butterfly kolam 8 by 8 dots</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/I_SIoefeXYA/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/I_SIoefeXYA</t>
+  </si>
+  <si>
+    <t>I_SIoefeXYA</t>
+  </si>
+  <si>
+    <t>Beautiful butterfly rangoli kolam |13*7 dots</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/XWralSEEXGI/mqdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/XWralSEEXGI</t>
+  </si>
+  <si>
+    <t>XWralSEEXGI</t>
   </si>
   <si>
     <t>ganesh chaturthi special rangoli design</t>
@@ -1949,90 +2036,6 @@
     <t>fuqzN6iCKoI</t>
   </si>
   <si>
-    <t>Beautiful Butterfly rangoli kolam |13*7 dots</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/sFyte69z454/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/sFyte69z454</t>
-  </si>
-  <si>
-    <t>sFyte69z454</t>
-  </si>
-  <si>
-    <t>simple butterfly kolam |13*7 dots</t>
-  </si>
-  <si>
-    <t>https://youtu.be/9JQVTQdqXS0</t>
-  </si>
-  <si>
-    <t>9JQVTQdqXS0</t>
-  </si>
-  <si>
-    <t>Rangoli Art | 7 to 4 Interlaced Dots</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/yzJ8lfMxlck/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/yzJ8lfMxlck</t>
-  </si>
-  <si>
-    <t>yzJ8lfMxlck</t>
-  </si>
-  <si>
-    <t>Simple Butterfly Rangoli Design with Colours &amp; dots 9x5</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/HnFDl171M4M/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/HnFDl171M4M</t>
-  </si>
-  <si>
-    <t>HnFDl171M4M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">simple flower rangoli with dots 12-2-2 </t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/KiCPCRXBOwo/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/KiCPCRXBOwo</t>
-  </si>
-  <si>
-    <t>KiCPCRXBOwo</t>
-  </si>
-  <si>
-    <t>Dheepiika Rangolis</t>
-  </si>
-  <si>
-    <t>butterfly kolam 8 by 8 dots</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/I_SIoefeXYA/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/I_SIoefeXYA</t>
-  </si>
-  <si>
-    <t>I_SIoefeXYA</t>
-  </si>
-  <si>
-    <t>Beautiful butterfly rangoli kolam |13*7 dots</t>
-  </si>
-  <si>
-    <t>https://i.ytimg.com/vi/XWralSEEXGI/mqdefault.jpg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/XWralSEEXGI</t>
-  </si>
-  <si>
-    <t>XWralSEEXGI</t>
-  </si>
-  <si>
     <t>Daily Rangoli Design With Colours and Dots 13x7</t>
   </si>
   <si>
@@ -2232,9 +2235,6 @@
   </si>
   <si>
     <t>JoOTT7Cwrs0</t>
-  </si>
-  <si>
-    <t>6wmY90tkzuI</t>
   </si>
   <si>
     <t>11 to 6 interlaced Dots - Easy Rangoli</t>
@@ -2460,13 +2460,13 @@
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF1155CC"/>
       <name val="Roboto"/>
     </font>
     <font>
       <u/>
-      <color rgb="FF1155CC"/>
+      <sz val="11.0"/>
+      <color rgb="FF0000FF"/>
       <name val="Roboto"/>
     </font>
     <font>
@@ -2567,10 +2567,10 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -2801,7 +2801,7 @@
       <c r="D4" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="9" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2819,7 +2819,7 @@
         <v>110</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6">
@@ -2836,7 +2836,7 @@
         <v>114</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7">
@@ -2853,7 +2853,7 @@
         <v>118</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8">
@@ -2938,7 +2938,7 @@
         <v>141</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -3023,7 +3023,7 @@
         <v>329</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3">
@@ -3040,7 +3040,7 @@
         <v>333</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4">
@@ -3057,7 +3057,7 @@
         <v>336</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5">
@@ -3099,7 +3099,7 @@
         <v>345</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>346</v>
@@ -3108,7 +3108,7 @@
         <v>347</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8">
@@ -3125,7 +3125,7 @@
         <v>351</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9">
@@ -3199,7 +3199,7 @@
         <v>390</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3">
@@ -3250,7 +3250,7 @@
         <v>402</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6">
@@ -3267,7 +3267,7 @@
         <v>406</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7">
@@ -3284,7 +3284,7 @@
         <v>410</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8">
@@ -3301,7 +3301,7 @@
         <v>414</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -3541,7 +3541,7 @@
         <v>418</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3">
@@ -3575,7 +3575,7 @@
         <v>427</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5">
@@ -3609,7 +3609,7 @@
         <v>436</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7">
@@ -3626,7 +3626,7 @@
         <v>440</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -3694,7 +3694,7 @@
         <v>472</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>473</v>
@@ -3705,7 +3705,7 @@
         <v>474</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>475</v>
@@ -3771,7 +3771,7 @@
         <v>485</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>486</v>
@@ -4054,7 +4054,7 @@
         <v>454</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5">
@@ -4505,36 +4505,36 @@
     </row>
     <row r="2" ht="16.5">
       <c r="A2" s="4" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>26</v>
+        <v>69</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>53</v>
+        <v>21</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4">
@@ -4599,7 +4599,7 @@
         <v>222</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>260</v>
+        <v>608</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>101</v>
@@ -4670,7 +4670,7 @@
         <v>402</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12">
@@ -5021,172 +5021,172 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" ht="16.5">
       <c r="A6" s="4" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>26</v>
+        <v>69</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>43</v>
+        <v>87</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -5253,50 +5253,50 @@
     </row>
     <row r="2">
       <c r="A2" s="10" t="s">
-        <v>608</v>
+        <v>637</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>609</v>
+        <v>638</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>610</v>
+        <v>639</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>611</v>
+        <v>640</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>612</v>
+        <v>641</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="10" t="s">
-        <v>613</v>
+        <v>642</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>614</v>
+        <v>643</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>615</v>
+        <v>644</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>616</v>
+        <v>645</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>617</v>
+        <v>646</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>618</v>
+        <v>647</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>619</v>
+        <v>648</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>620</v>
+        <v>649</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>146</v>
@@ -5304,70 +5304,70 @@
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
-        <v>621</v>
+        <v>650</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>622</v>
+        <v>651</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>623</v>
+        <v>652</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>624</v>
+        <v>653</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="10" t="s">
-        <v>625</v>
+        <v>654</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>626</v>
+        <v>655</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>627</v>
+        <v>656</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>628</v>
+        <v>657</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
-        <v>629</v>
+        <v>658</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>630</v>
+        <v>659</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>631</v>
+        <v>660</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>632</v>
+        <v>661</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>633</v>
+        <v>662</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="10" t="s">
-        <v>634</v>
+        <v>663</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>507</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>635</v>
+        <v>664</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>636</v>
+        <v>665</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>633</v>
+        <v>662</v>
       </c>
     </row>
   </sheetData>
@@ -5423,16 +5423,16 @@
     </row>
     <row r="2">
       <c r="A2" s="10" t="s">
-        <v>637</v>
+        <v>609</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>638</v>
+        <v>610</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>639</v>
+        <v>611</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>640</v>
+        <v>612</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>423</v>
@@ -5440,16 +5440,16 @@
     </row>
     <row r="3">
       <c r="A3" s="10" t="s">
-        <v>641</v>
+        <v>613</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>510</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>642</v>
+        <v>614</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>643</v>
+        <v>615</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>423</v>
@@ -5457,16 +5457,16 @@
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>644</v>
+        <v>616</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>645</v>
+        <v>617</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>646</v>
+        <v>618</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>101</v>
@@ -5474,16 +5474,16 @@
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
-        <v>648</v>
+        <v>620</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>649</v>
+        <v>621</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>650</v>
+        <v>622</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>651</v>
+        <v>623</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>146</v>
@@ -5491,33 +5491,33 @@
     </row>
     <row r="6">
       <c r="A6" s="10" t="s">
-        <v>652</v>
+        <v>624</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>653</v>
+        <v>625</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>654</v>
+        <v>626</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>655</v>
+        <v>627</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>656</v>
+        <v>628</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
-        <v>657</v>
+        <v>629</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>658</v>
+        <v>630</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>659</v>
+        <v>631</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>660</v>
+        <v>632</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>155</v>
@@ -5525,16 +5525,16 @@
     </row>
     <row r="8">
       <c r="A8" s="10" t="s">
-        <v>661</v>
+        <v>633</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>662</v>
+        <v>634</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>663</v>
+        <v>635</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>664</v>
+        <v>636</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>423</v>
@@ -5594,16 +5594,16 @@
     </row>
     <row r="2">
       <c r="A2" s="10" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>146</v>
@@ -5611,33 +5611,33 @@
     </row>
     <row r="3">
       <c r="A3" s="10" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>513</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>423</v>
@@ -5645,16 +5645,16 @@
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>423</v>
@@ -5662,16 +5662,16 @@
     </row>
     <row r="6">
       <c r="A6" s="10" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>423</v>
@@ -5679,33 +5679,33 @@
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="10" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>101</v>
@@ -5713,16 +5713,16 @@
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>101</v>
@@ -5784,41 +5784,41 @@
     </row>
     <row r="2">
       <c r="A2" s="10" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="10" t="s">
+        <v>704</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>705</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>706</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>707</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>703</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>704</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>705</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>706</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>256</v>
@@ -5835,19 +5835,19 @@
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6">
@@ -5869,16 +5869,16 @@
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>178</v>
@@ -5898,24 +5898,24 @@
         <v>402</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>516</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -5974,16 +5974,16 @@
     </row>
     <row r="2">
       <c r="A2" s="10" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>259</v>
@@ -5991,36 +5991,36 @@
     </row>
     <row r="3">
       <c r="A3" s="10" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5">
@@ -6034,7 +6034,7 @@
         <v>222</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>732</v>
+        <v>260</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>101</v>
@@ -6071,7 +6071,7 @@
         <v>740</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
     </row>
     <row r="8">
@@ -6088,7 +6088,7 @@
         <v>743</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -6173,7 +6173,7 @@
         <v>333</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4">
@@ -6190,7 +6190,7 @@
         <v>753</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5">
@@ -6207,7 +6207,7 @@
         <v>756</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6">
@@ -6241,7 +6241,7 @@
         <v>765</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8">
@@ -6258,7 +6258,7 @@
         <v>197</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -6326,7 +6326,7 @@
         <v>772</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3">
@@ -6360,7 +6360,7 @@
         <v>780</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5">
@@ -6466,172 +6466,172 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>53</v>
+        <v>13</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>53</v>
+        <v>17</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>53</v>
+        <v>21</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>53</v>
+        <v>25</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>70</v>
+        <v>26</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>71</v>
+        <v>27</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>53</v>
+        <v>29</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>74</v>
+        <v>30</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>76</v>
+        <v>32</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>78</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>81</v>
+        <v>37</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>82</v>
+        <v>38</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" ht="16.5">
       <c r="A10" s="4" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>85</v>
+        <v>42</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>87</v>
+        <v>43</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>88</v>
+        <v>45</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>90</v>
+        <v>47</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>87</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14">
@@ -6748,7 +6748,7 @@
         <v>185</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5">
@@ -6782,7 +6782,7 @@
         <v>193</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7">
@@ -6799,7 +6799,7 @@
         <v>197</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8">
@@ -6849,7 +6849,7 @@
       <c r="D10" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>101</v>
       </c>
     </row>
@@ -6866,12 +6866,12 @@
       <c r="D11" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="8" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="12">
-      <c r="E12" s="9"/>
+      <c r="E12" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -7038,7 +7038,7 @@
         <v>169</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8">
@@ -7225,7 +7225,7 @@
         <v>240</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9">
@@ -7313,7 +7313,7 @@
         <v>249</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3">
@@ -7464,7 +7464,7 @@
         <v>273</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3">
@@ -7560,10 +7560,10 @@
         <v>297</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>283</v>
@@ -7626,7 +7626,7 @@
         <v>274</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>301</v>
@@ -7669,7 +7669,7 @@
         <v>311</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>78</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5">

</xml_diff>